<commit_message>
add/ zephyr mobile app
</commit_message>
<xml_diff>
--- a/zephyrm-backend/files/assets_report.xlsx
+++ b/zephyrm-backend/files/assets_report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="22">
   <si>
     <t>Title</t>
   </si>
@@ -46,22 +46,37 @@
     <t>Cordoba</t>
   </si>
   <si>
-    <t>Free</t>
+    <t>On loan</t>
   </si>
   <si>
-    <t>Prueba</t>
+    <t>Pruebacion portas</t>
   </si>
   <si>
     <t>Unassigned</t>
   </si>
   <si>
+    <t>Jose Cabrera</t>
+  </si>
+  <si>
+    <t>Free</t>
+  </si>
+  <si>
     <t>Carlos</t>
   </si>
   <si>
-    <t>Jose Cabrera</t>
+    <t xml:space="preserve">teresa saez </t>
   </si>
   <si>
-    <t>PruebaAdmin</t>
+    <t>gatos</t>
+  </si>
+  <si>
+    <t>mascotas</t>
+  </si>
+  <si>
+    <t>animal blanquito y suave</t>
+  </si>
+  <si>
+    <t>Under maintenance</t>
   </si>
 </sst>
 </file>
@@ -414,10 +429,10 @@
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="8" width="22" customWidth="1"/>
     <col min="9" max="26" width="10" customWidth="1"/>
   </cols>
   <sheetData>
@@ -536,7 +551,7 @@
         <v>11</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -556,7 +571,7 @@
         <v>10</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>13</v>
@@ -582,7 +597,7 @@
         <v>11</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
@@ -602,7 +617,7 @@
         <v>10</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>13</v>
@@ -625,7 +640,7 @@
         <v>10</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>13</v>
@@ -648,7 +663,7 @@
         <v>10</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>13</v>
@@ -674,7 +689,7 @@
         <v>11</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
@@ -697,7 +712,7 @@
         <v>11</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
@@ -717,7 +732,7 @@
         <v>10</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>13</v>
@@ -743,15 +758,31 @@
         <v>11</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="2"/>
+      <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="7">
+        <v>45798.68992181713</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>

</xml_diff>